<commit_message>
wip: screen transition animations
</commit_message>
<xml_diff>
--- a/notes quotation-automator.xlsx
+++ b/notes quotation-automator.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="6450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="6450" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
     <sheet name="collections" sheetId="3" r:id="rId2"/>
     <sheet name="UI" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Development Time Reqd" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>v 0.1</t>
   </si>
@@ -90,16 +90,83 @@
   </si>
   <si>
     <t>text area text</t>
+  </si>
+  <si>
+    <t>Total 11 Skide</t>
+  </si>
+  <si>
+    <t>Animation Tut</t>
+  </si>
+  <si>
+    <t>App Master State</t>
+  </si>
+  <si>
+    <t>Slide-1 UI and State/Props</t>
+  </si>
+  <si>
+    <t>Slide 2</t>
+  </si>
+  <si>
+    <t>Slide 3</t>
+  </si>
+  <si>
+    <t>Slide 4</t>
+  </si>
+  <si>
+    <t>Slide 5</t>
+  </si>
+  <si>
+    <t>Slide 6</t>
+  </si>
+  <si>
+    <t>Slide 7</t>
+  </si>
+  <si>
+    <t>Slide 8</t>
+  </si>
+  <si>
+    <t>Slide 9</t>
+  </si>
+  <si>
+    <t>Slide 10</t>
+  </si>
+  <si>
+    <t>Slide 11</t>
+  </si>
+  <si>
+    <t>Calculating cost for each door property, .75 x 9</t>
+  </si>
+  <si>
+    <t>Display Final</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>x 3 as per Dev Mastery</t>
+  </si>
+  <si>
+    <t>No of Hrs</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>1 month on 2 hrs per day
+Start Date: 03-10-2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,8 +190,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +221,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -188,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -220,6 +301,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,12 +937,193 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6.75</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="21">
+        <f>SUM(C2:C16)</f>
+        <v>15.25</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="21">
+        <f>C17*3</f>
+        <v>45.75</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
wip: slide in out animation
</commit_message>
<xml_diff>
--- a/notes quotation-automator.xlsx
+++ b/notes quotation-automator.xlsx
@@ -17,7 +17,7 @@
     <sheet name="UI" sheetId="2" r:id="rId3"/>
     <sheet name="Development Time Reqd" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -92,9 +92,6 @@
     <t>text area text</t>
   </si>
   <si>
-    <t>Total 11 Skide</t>
-  </si>
-  <si>
     <t>Animation Tut</t>
   </si>
   <si>
@@ -157,12 +154,15 @@
   <si>
     <t>1 month on 2 hrs per day
 Start Date: 03-10-2017</t>
+  </si>
+  <si>
+    <t>Total 11 Slide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -940,7 +940,7 @@
   <dimension ref="B1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,30 +953,30 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -985,7 +985,7 @@
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1">
         <v>0.5</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1">
         <v>0.5</v>
@@ -1012,7 +1012,7 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1">
         <v>0.5</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1">
         <v>0.5</v>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1">
         <v>0.5</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1">
         <v>0.5</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1">
         <v>0.5</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1">
         <v>0.5</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1">
         <v>0.5</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1">
         <v>0.5</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1">
         <v>6.75</v>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1">
         <v>0.5</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="17" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="21">
         <f>SUM(C2:C16)</f>
@@ -1112,14 +1112,14 @@
     </row>
     <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="21">
         <f>C17*3</f>
         <v>45.75</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated presentation, have to make a production quality app
</commit_message>
<xml_diff>
--- a/notes quotation-automator.xlsx
+++ b/notes quotation-automator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="6450" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="6450"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
     <t>Misc</t>
   </si>
   <si>
-    <t>Progress Bar on top</t>
-  </si>
-  <si>
     <t>quote</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>Total 11 Slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Redux to Store </t>
   </si>
 </sst>
 </file>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +620,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -808,87 +808,87 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -939,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -953,30 +953,30 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>39</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -985,7 +985,7 @@
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1">
         <v>0.5</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1">
         <v>0.5</v>
@@ -1012,7 +1012,7 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1">
         <v>0.5</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1">
         <v>0.5</v>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1">
         <v>0.5</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1">
         <v>0.5</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1">
         <v>0.5</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1">
         <v>0.5</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1">
         <v>0.5</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1">
         <v>0.5</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1">
         <v>6.75</v>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1">
         <v>0.5</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="17" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="21">
         <f>SUM(C2:C16)</f>
@@ -1112,14 +1112,14 @@
     </row>
     <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="21">
         <f>C17*3</f>
         <v>45.75</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>